<commit_message>
Forms SOPs 1 & 2
</commit_message>
<xml_diff>
--- a/1-Software Development Lifecycle/Forms/Bug Form - F7.xlsx
+++ b/1-Software Development Lifecycle/Forms/Bug Form - F7.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayed.hawas\Downloads\3-12-2025\SW 2025\SW 2025\1-Software Development Lifecycle\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heba.backar\Downloads\SW 2025 2\SW 2025\SW 2025\1-Software Development Lifecycle\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF08317-8E7B-44E3-9FCC-4BF0861F0C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A660EF2-0AAB-42DB-A712-132389E982F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0FD72531-45CD-44DA-85CA-64CA552C7522}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FD72531-45CD-44DA-85CA-64CA552C7522}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="F-SW-SD-07" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'F-SW-SD-07'!$A$1:$F$18</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -299,27 +299,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -329,9 +365,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -340,39 +373,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,8 +746,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,36 +760,36 @@
     <row r="1" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -797,10 +797,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -808,30 +808,30 @@
         <v>2</v>
       </c>
       <c r="B7" s="10"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="26" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -843,10 +843,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="10"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -854,32 +854,32 @@
         <v>19</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -931,28 +931,31 @@
         <v>28</v>
       </c>
       <c r="B18" s="10"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
     </row>
     <row r="19" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:F6"/>
@@ -961,22 +964,19 @@
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C15:F15"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C12:F12"/>
-    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select your department from the drop list" sqref="C9:F9" xr:uid="{937FC6FA-E998-404A-A948-19D40203D519}"/>

</xml_diff>